<commit_message>
implement payment management functionality, including a custom calendar control and associated view models.
</commit_message>
<xml_diff>
--- a/src/backend/VoltStream.Infrastructure/SeedData/Users.xlsx
+++ b/src/backend/VoltStream.Infrastructure/SeedData/Users.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Username</t>
   </si>
@@ -58,6 +58,21 @@
   </si>
   <si>
     <t xml:space="preserve">Farg'ona, O'zbekiston</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>Boshqaruvchi</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+998 91 6554321</t>
+  </si>
+  <si>
+    <t>manager@voltstream.uz</t>
   </si>
 </sst>
 </file>
@@ -70,13 +85,12 @@
   <fonts count="4">
     <font>
       <sz val="10.000000"/>
-      <color indexed="64"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10.000000"/>
-      <color indexed="64"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -682,7 +696,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="1">
-        <v>123</v>
+        <v>8520</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -704,20 +718,37 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+    <row r="3" ht="25.5">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1">
+        <v>123</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="4">
+        <v>35998</v>
+      </c>
       <c r="I3" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="F2"/>
+    <hyperlink r:id="rId2" ref="F3"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
add admin lock overlay & JWT auth for settings protection
</commit_message>
<xml_diff>
--- a/src/backend/VoltStream.Infrastructure/SeedData/Users.xlsx
+++ b/src/backend/VoltStream.Infrastructure/SeedData/Users.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Username</t>
   </si>
@@ -42,6 +42,15 @@
     <t>DateOfBirth</t>
   </si>
   <si>
+    <t>IsActive</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>TimeZone</t>
+  </si>
+  <si>
     <t>admin</t>
   </si>
   <si>
@@ -58,6 +67,9 @@
   </si>
   <si>
     <t xml:space="preserve">Farg'ona, O'zbekiston</t>
+  </si>
+  <si>
+    <t>Male</t>
   </si>
   <si>
     <t>manager</t>
@@ -140,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -156,6 +168,8 @@
     <xf fontId="1" fillId="0" borderId="1" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="0" wrapText="1"/>
     </xf>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,61 +703,85 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2"/>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" ht="25.5">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1">
         <v>8520</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H2" s="4">
         <v>35998</v>
       </c>
-      <c r="I2" s="2"/>
+      <c r="I2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" ht="25.5">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1">
         <v>123</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="H3" s="4">
         <v>35998</v>
       </c>
-      <c r="I3" s="2"/>
+      <c r="I3" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>